<commit_message>
add check for water and electro
add check for water and electro
</commit_message>
<xml_diff>
--- a/Інфо_борги.xlsx
+++ b/Інфо_борги.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="212">
   <si>
     <t>Під’їзд</t>
   </si>
@@ -663,6 +663,9 @@
   </si>
   <si>
     <t>курс долара</t>
+  </si>
+  <si>
+    <t>70%від вартості іконостасу (30000 $) погашено</t>
   </si>
 </sst>
 </file>
@@ -1353,8 +1356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M212"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="F172" sqref="F172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,6 +1366,7 @@
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="48.85546875" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="55.5703125" customWidth="1"/>
     <col min="11" max="11" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3643,7 +3647,7 @@
         <v>-371.24</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="29"/>
       <c r="B161" s="31"/>
       <c r="C161" s="5">
@@ -3656,7 +3660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="29"/>
       <c r="B162" s="31"/>
       <c r="C162" s="5">
@@ -3669,7 +3673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="29"/>
       <c r="B163" s="31"/>
       <c r="C163" s="5">
@@ -3682,7 +3686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="29"/>
       <c r="B164" s="31" t="s">
         <v>11</v>
@@ -3697,7 +3701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="29"/>
       <c r="B165" s="31"/>
       <c r="C165" s="5">
@@ -3710,7 +3714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="29"/>
       <c r="B166" s="31"/>
       <c r="C166" s="5">
@@ -3723,7 +3727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="29"/>
       <c r="B167" s="31"/>
       <c r="C167" s="5">
@@ -3736,7 +3740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="29"/>
       <c r="B168" s="31"/>
       <c r="C168" s="5">
@@ -3749,7 +3753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="29"/>
       <c r="B169" s="31"/>
       <c r="C169" s="5">
@@ -3761,8 +3765,11 @@
       <c r="E169" s="15">
         <v>19400</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F169" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="29"/>
       <c r="B170" s="31">
         <v>4</v>
@@ -3777,7 +3784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="29"/>
       <c r="B171" s="31"/>
       <c r="C171" s="5">
@@ -3789,8 +3796,11 @@
       <c r="E171" s="15">
         <v>13503.39</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F171" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="29"/>
       <c r="B172" s="31"/>
       <c r="C172" s="5">
@@ -3803,7 +3813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="29"/>
       <c r="B173" s="31"/>
       <c r="C173" s="5">
@@ -3816,7 +3826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="29"/>
       <c r="B174" s="31"/>
       <c r="C174" s="5">
@@ -3829,7 +3839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="29"/>
       <c r="B175" s="31"/>
       <c r="C175" s="5">
@@ -3842,7 +3852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="29"/>
       <c r="B176" s="31">
         <v>5</v>

</xml_diff>